<commit_message>
add another PA group
</commit_message>
<xml_diff>
--- a/010_data/2020_PA.xlsx
+++ b/010_data/2020_PA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/Hanks-Research/2020_Kestrel_Plots/010_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A18B58E-78CD-BE4D-B99F-CCCBAADE4012}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F562C2CF-BE73-2A49-B24F-C8C0A624DC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="460" windowWidth="27400" windowHeight="17040" xr2:uid="{FBB681FB-660C-454A-A7AE-1280157312B2}"/>
+    <workbookView xWindow="6120" yWindow="920" windowWidth="27400" windowHeight="17040" xr2:uid="{FBB681FB-660C-454A-A7AE-1280157312B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t># chicks</t>
   </si>
@@ -89,14 +89,17 @@
     <t>year</t>
   </si>
   <si>
-    <t>Devich Farbotnik in Bucks County, PA</t>
+    <t>Devich Farbotnik in Bucks County</t>
+  </si>
+  <si>
+    <t>Jere Schade and Steve Benningfield in Bucks County</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -114,6 +117,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,10 +148,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9474FD0B-C36E-E645-A63D-D7F861907EC9}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -482,7 +492,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
@@ -496,7 +506,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -510,7 +520,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -524,7 +534,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -538,7 +548,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -552,7 +562,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -566,7 +576,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -580,7 +590,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -594,7 +604,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="2">
@@ -608,7 +618,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="2">
@@ -622,7 +632,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2">
@@ -636,7 +646,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="2">
@@ -650,7 +660,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="2">
@@ -664,7 +674,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="2">
@@ -678,7 +688,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="2">
@@ -689,6 +699,76 @@
       </c>
       <c r="D16" s="2">
         <v>3.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2016</v>
+      </c>
+      <c r="C17" s="2">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C18" s="2">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C19" s="2">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C20" s="2">
+        <v>18</v>
+      </c>
+      <c r="D20" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C21" s="2">
+        <v>37</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more PA data, expand axes, rerun all
</commit_message>
<xml_diff>
--- a/010_data/2020_PA.xlsx
+++ b/010_data/2020_PA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/Hanks-Research/2020_Kestrel_Plots/010_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F562C2CF-BE73-2A49-B24F-C8C0A624DC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F72DFC3-828C-BF4D-AC99-1B78159780FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="920" windowWidth="27400" windowHeight="17040" xr2:uid="{FBB681FB-660C-454A-A7AE-1280157312B2}"/>
+    <workbookView xWindow="1400" yWindow="920" windowWidth="27400" windowHeight="17040" xr2:uid="{FBB681FB-660C-454A-A7AE-1280157312B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t># chicks</t>
   </si>
@@ -41,9 +41,6 @@
     <t>chicks/nested box</t>
   </si>
   <si>
-    <t xml:space="preserve">PA Shaver’s Cr SE   </t>
-  </si>
-  <si>
     <t>2019                 </t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>294                                     </t>
   </si>
   <si>
-    <t xml:space="preserve">PA Shaver’s Cr JK </t>
-  </si>
-  <si>
     <t>12                                        </t>
   </si>
   <si>
@@ -93,13 +87,25 @@
   </si>
   <si>
     <t>Jere Schade and Steve Benningfield in Bucks County</t>
+  </si>
+  <si>
+    <t>PA Game Commission SE</t>
+  </si>
+  <si>
+    <t>PA Shaver’s Creek</t>
+  </si>
+  <si>
+    <t>Eisenhauer</t>
+  </si>
+  <si>
+    <t>Hawk Mountain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,6 +133,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -148,11 +166,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9474FD0B-C36E-E645-A63D-D7F861907EC9}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -482,7 +502,7 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -493,7 +513,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2">
         <v>2018</v>
@@ -507,13 +527,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="D3" s="2">
         <v>3.9</v>
@@ -521,13 +541,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="D4" s="2">
         <v>4.0999999999999996</v>
@@ -535,13 +555,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2">
         <v>2.4</v>
@@ -549,13 +569,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
         <v>1.8</v>
@@ -563,13 +583,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2">
         <v>3.3</v>
@@ -577,13 +597,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2">
         <v>3.5</v>
@@ -591,13 +611,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2">
         <v>3.7</v>
@@ -605,7 +625,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2">
         <v>2014</v>
@@ -619,7 +639,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2">
         <v>2015</v>
@@ -633,7 +653,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2">
         <v>2016</v>
@@ -647,7 +667,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2">
         <v>2017</v>
@@ -661,7 +681,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2">
         <v>2018</v>
@@ -675,7 +695,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2">
         <v>2019</v>
@@ -689,7 +709,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2">
         <v>2020</v>
@@ -703,7 +723,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
         <v>2016</v>
@@ -717,7 +737,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2">
         <v>2017</v>
@@ -731,7 +751,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>2018</v>
@@ -745,7 +765,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2">
         <v>2019</v>
@@ -759,7 +779,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2">
         <v>2020</v>
@@ -769,6 +789,242 @@
       </c>
       <c r="D21" s="2">
         <v>3.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C22" s="4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C23" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C24" s="4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C25" s="4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2016</v>
+      </c>
+      <c r="C26" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2015</v>
+      </c>
+      <c r="C27" s="4">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C28" s="4">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C29" s="4">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2012</v>
+      </c>
+      <c r="C30" s="4">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2011</v>
+      </c>
+      <c r="C31" s="4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2012</v>
+      </c>
+      <c r="C32" s="2">
+        <v>34</v>
+      </c>
+      <c r="D32" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C33" s="2">
+        <v>58</v>
+      </c>
+      <c r="D33" s="2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C34" s="2">
+        <v>53</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2015</v>
+      </c>
+      <c r="C35" s="2">
+        <v>58</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2016</v>
+      </c>
+      <c r="C36" s="2">
+        <v>63</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C37" s="2">
+        <v>86</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C38" s="2">
+        <v>110</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C39" s="2">
+        <v>170</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C40" s="2">
+        <v>226</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>